<commit_message>
Template fix and svg file
</commit_message>
<xml_diff>
--- a/website/static/assets/metadata_template.xlsx
+++ b/website/static/assets/metadata_template.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tushar/PDX/pdxfinder-data/template/active_templates/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tushar/CancerModels/sa-y3/pdcm-submission/website/static/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004EF1B4-CD4F-5248-902F-60EE79FB296C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F823A71-C97C-074A-B0BA-8B838611F812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35720" yWindow="500" windowWidth="33600" windowHeight="19880" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19260" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient" sheetId="1" r:id="rId1"/>
     <sheet name="patient_sample" sheetId="2" r:id="rId2"/>
-    <sheet name="pdx_models" sheetId="3" r:id="rId3"/>
+    <sheet name="pdx_model" sheetId="3" r:id="rId3"/>
     <sheet name="model_validation" sheetId="4" r:id="rId4"/>
     <sheet name="cell_model" sheetId="6" r:id="rId5"/>
     <sheet name="sharing" sheetId="5" r:id="rId6"/>
@@ -3430,7 +3430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK982"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -4722,7 +4722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6038AA-9EAD-E846-B5BE-A0ADCFA2926F}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>